<commit_message>
Certificate Assignment has been Done
</commit_message>
<xml_diff>
--- a/User Assignment Mapping.xlsx
+++ b/User Assignment Mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dadu\Desktop\New folder (3)\certificate-assignments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Snehal\study Snehal\Full Stack\Assignment\certificate-assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D35475B-C1DE-4376-A1D8-98B98FC766E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBE98EE-1595-4F0E-B168-330577088B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="272">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -841,6 +832,15 @@
   </si>
   <si>
     <t>rutujaganjure07@gmail.com</t>
+  </si>
+  <si>
+    <t>Snehal</t>
+  </si>
+  <si>
+    <t>More</t>
+  </si>
+  <si>
+    <t>snewrk30@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1493,8 +1493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="83" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="83" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M74" sqref="M74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2149,7 +2149,7 @@
       </c>
       <c r="G32" s="15"/>
     </row>
-    <row r="33" spans="1:10" ht="27">
+    <row r="33" spans="1:10">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2731,9 +2731,15 @@
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="B65" s="4"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="25"/>
+      <c r="B65" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>271</v>
+      </c>
       <c r="E65" t="str">
         <f t="shared" si="3"/>
         <v>designs/78.jpg</v>
@@ -4425,10 +4431,11 @@
     <hyperlink ref="D122" r:id="rId30" xr:uid="{B8DC8EDA-D092-4793-BA05-95C74E6867C5}"/>
     <hyperlink ref="D123" r:id="rId31" xr:uid="{E07B5D07-9ACB-475C-9DA7-9296F65D260C}"/>
     <hyperlink ref="D48" r:id="rId32" xr:uid="{96BF6809-7913-4933-AE65-A1CC94949B04}"/>
+    <hyperlink ref="D65" r:id="rId33" xr:uid="{407EDCA2-929D-4B8E-9294-2A0B869967E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId33"/>
+    <tablePart r:id="rId34"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>